<commit_message>
Aufteilung in Main und Betriebstag.py
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -11,6 +11,10 @@
     <sheet name="Umlauf Nr. 2" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Umlauf Nr. 3" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Umlauf Nr. 4" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Umlauf Nr. 11" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Umlauf Nr. 21" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Umlauf Nr. 31" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Umlauf Nr. 41" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -2665,4 +2669,2252 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Zeit [s]</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>SoC [%]</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Zurückgelegte Distanz [m]</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Ist-Geschwindigkeit zum Zeitpunkt t [m/s]</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Soll-Geschwindigkeit zum Zeitpunkt t [m/s]</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Steigung im Intervall [t, t+1) [%]</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Gewählte Beschleunigung im Intervall [t, t+1) [m/s²]</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Abgerufene Batterieleistung im Intervall [t, t+1) [W]</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Kumulierter Energieverbrauch nach Intervall [t, t+1) [kWh]</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>37.89473684210527</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1.052631578947369e-05</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>99.9999969924812</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.5144032921810699</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.02880658436214</v>
+      </c>
+      <c r="E3" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>17019.3250964519</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.004738116620359448</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>99.99864625239418</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.05761316872428</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2.05761316872428</v>
+      </c>
+      <c r="E4" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>34013.11198130637</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.01418620328183344</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>99.99594679906232</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4.62962962962963</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3.08641975308642</v>
+      </c>
+      <c r="E5" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>51031.61191665019</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.02836165103645849</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>99.99189667113244</v>
+      </c>
+      <c r="C6" t="n">
+        <v>8.230452674897119</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4.11522633744856</v>
+      </c>
+      <c r="E6" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>64688.6404626334</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.04633071783163444</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>99.98676265204811</v>
+      </c>
+      <c r="C7" t="n">
+        <v>12.86008230452675</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5.1440329218107</v>
+      </c>
+      <c r="E7" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>80944.00083341627</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.06881516250758339</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>99.98033852499783</v>
+      </c>
+      <c r="C8" t="n">
+        <v>18.51851851851852</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6.17283950617284</v>
+      </c>
+      <c r="E8" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.9716506630086876</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>92309.36376947795</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.09445665244354949</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>99.97301238501612</v>
+      </c>
+      <c r="C9" t="n">
+        <v>25.17718335619571</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7.144490169181528</v>
+      </c>
+      <c r="E9" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0.8816830090264018</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>97987.04144175485</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.1216752750662592</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>99.96523563569536</v>
+      </c>
+      <c r="C10" t="n">
+        <v>32.76251502989044</v>
+      </c>
+      <c r="D10" t="n">
+        <v>8.02617317820793</v>
+      </c>
+      <c r="E10" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0.8000456933758091</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>101081.4420481137</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.1497534534129574</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>99.95721329902489</v>
+      </c>
+      <c r="C11" t="n">
+        <v>41.18871105478627</v>
+      </c>
+      <c r="D11" t="n">
+        <v>8.826218871583739</v>
+      </c>
+      <c r="E11" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0.7442224083688047</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>104463.2727333196</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.1787710291722129</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>99.94892256309366</v>
+      </c>
+      <c r="C12" t="n">
+        <v>50.38704113055441</v>
+      </c>
+      <c r="D12" t="n">
+        <v>9.570441279952544</v>
+      </c>
+      <c r="E12" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>0.7028767190149822</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>67147.86387781269</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.1974232135827164</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>99.94359336754781</v>
+      </c>
+      <c r="C13" t="n">
+        <v>60.30892077001444</v>
+      </c>
+      <c r="D13" t="n">
+        <v>10.27331799896753</v>
+      </c>
+      <c r="E13" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>0.6638280124030387</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>65305.45819627993</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.2155636186372386</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>99.93841039467509</v>
+      </c>
+      <c r="C14" t="n">
+        <v>70.91415277518348</v>
+      </c>
+      <c r="D14" t="n">
+        <v>10.93714601137057</v>
+      </c>
+      <c r="E14" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0.6269486783806476</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>151428.2202920164</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.2576270131627987</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>99.9263922819535</v>
+      </c>
+      <c r="C15" t="n">
+        <v>82.16477312574438</v>
+      </c>
+      <c r="D15" t="n">
+        <v>11.56409468975121</v>
+      </c>
+      <c r="E15" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>0.6091420889097003</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>157524.8125526304</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.3013839055385293</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>99.9138903127033</v>
+      </c>
+      <c r="C16" t="n">
+        <v>94.03343885995044</v>
+      </c>
+      <c r="D16" t="n">
+        <v>12.17323677866091</v>
+      </c>
+      <c r="E16" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F16" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>0.598193456592696</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>224426.0499971094</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.3637244749821708</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>99.8960787214337</v>
+      </c>
+      <c r="C17" t="n">
+        <v>106.5057723669077</v>
+      </c>
+      <c r="D17" t="n">
+        <v>12.77143023525361</v>
+      </c>
+      <c r="E17" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F17" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>0.5874416134186443</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>254838.62966634</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.4345129832228208</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Zeit [s]</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>SoC [%]</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Zurückgelegte Distanz [m]</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Ist-Geschwindigkeit zum Zeitpunkt t [m/s]</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Soll-Geschwindigkeit zum Zeitpunkt t [m/s]</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Steigung im Intervall [t, t+1) [%]</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Gewählte Beschleunigung im Intervall [t, t+1) [m/s²]</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Abgerufene Batterieleistung im Intervall [t, t+1) [W]</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Kumulierter Energieverbrauch nach Intervall [t, t+1) [kWh]</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>99.87585343336495</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>37.89473684210527</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1.052631578947369e-05</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>99.87585042584615</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.5144032921810699</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.02880658436214</v>
+      </c>
+      <c r="E3" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>17019.3250964519</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.004738116620359448</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>99.87449968575913</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.05761316872428</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2.05761316872428</v>
+      </c>
+      <c r="E4" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>34013.11198130637</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.01418620328183344</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>99.87180023242729</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4.62962962962963</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3.08641975308642</v>
+      </c>
+      <c r="E5" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>51031.61191665019</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.02836165103645849</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>99.8677501044974</v>
+      </c>
+      <c r="C6" t="n">
+        <v>8.230452674897119</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4.11522633744856</v>
+      </c>
+      <c r="E6" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>64688.6404626334</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.04633071783163444</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>99.86261608541307</v>
+      </c>
+      <c r="C7" t="n">
+        <v>12.86008230452675</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5.1440329218107</v>
+      </c>
+      <c r="E7" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>80944.00083341627</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.06881516250758339</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>99.8561919583628</v>
+      </c>
+      <c r="C8" t="n">
+        <v>18.51851851851852</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6.17283950617284</v>
+      </c>
+      <c r="E8" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.9716506630086876</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>92309.36376947795</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.09445665244354949</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>99.84886581838109</v>
+      </c>
+      <c r="C9" t="n">
+        <v>25.17718335619571</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7.144490169181528</v>
+      </c>
+      <c r="E9" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0.8816830090264018</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>97987.04144175485</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.1216752750662592</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>99.84108906906032</v>
+      </c>
+      <c r="C10" t="n">
+        <v>32.76251502989044</v>
+      </c>
+      <c r="D10" t="n">
+        <v>8.02617317820793</v>
+      </c>
+      <c r="E10" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0.8000456933758091</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>101081.4420481137</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.1497534534129574</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>99.83306673238984</v>
+      </c>
+      <c r="C11" t="n">
+        <v>41.18871105478627</v>
+      </c>
+      <c r="D11" t="n">
+        <v>8.826218871583739</v>
+      </c>
+      <c r="E11" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0.7442224083688047</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>104463.2727333196</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.1787710291722129</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>99.82477599645861</v>
+      </c>
+      <c r="C12" t="n">
+        <v>50.38704113055441</v>
+      </c>
+      <c r="D12" t="n">
+        <v>9.570441279952544</v>
+      </c>
+      <c r="E12" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>0.7028767190149822</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>67147.86387781269</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.1974232135827164</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>99.81944680091276</v>
+      </c>
+      <c r="C13" t="n">
+        <v>60.30892077001444</v>
+      </c>
+      <c r="D13" t="n">
+        <v>10.27331799896753</v>
+      </c>
+      <c r="E13" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>0.6638280124030387</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>65305.45819627993</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.2155636186372386</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>99.81426382804005</v>
+      </c>
+      <c r="C14" t="n">
+        <v>70.91415277518348</v>
+      </c>
+      <c r="D14" t="n">
+        <v>10.93714601137057</v>
+      </c>
+      <c r="E14" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0.6269486783806476</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>151428.2202920164</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.2576270131627987</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>99.80224571531846</v>
+      </c>
+      <c r="C15" t="n">
+        <v>82.16477312574438</v>
+      </c>
+      <c r="D15" t="n">
+        <v>11.56409468975121</v>
+      </c>
+      <c r="E15" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>0.6091420889097003</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>157524.8125526304</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.3013839055385293</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>99.78974374606825</v>
+      </c>
+      <c r="C16" t="n">
+        <v>94.03343885995044</v>
+      </c>
+      <c r="D16" t="n">
+        <v>12.17323677866091</v>
+      </c>
+      <c r="E16" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F16" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>0.598193456592696</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>224426.0499971094</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.3637244749821708</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>99.77193215479866</v>
+      </c>
+      <c r="C17" t="n">
+        <v>106.5057723669077</v>
+      </c>
+      <c r="D17" t="n">
+        <v>12.77143023525361</v>
+      </c>
+      <c r="E17" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F17" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>0.5874416134186443</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>254838.62966634</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.4345129832228208</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Zeit [s]</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>SoC [%]</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Zurückgelegte Distanz [m]</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Ist-Geschwindigkeit zum Zeitpunkt t [m/s]</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Soll-Geschwindigkeit zum Zeitpunkt t [m/s]</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Steigung im Intervall [t, t+1) [%]</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Gewählte Beschleunigung im Intervall [t, t+1) [m/s²]</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Abgerufene Batterieleistung im Intervall [t, t+1) [W]</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Kumulierter Energieverbrauch nach Intervall [t, t+1) [kWh]</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>99.7517068667299</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>37.89473684210527</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1.052631578947369e-05</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>99.75170385921109</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.5144032921810699</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.02880658436214</v>
+      </c>
+      <c r="E3" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>17019.3250964519</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.004738116620359448</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>99.75035311912409</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.05761316872428</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2.05761316872428</v>
+      </c>
+      <c r="E4" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>34013.11198130637</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.01418620328183344</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>99.74765366579223</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4.62962962962963</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3.08641975308642</v>
+      </c>
+      <c r="E5" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>51031.61191665019</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.02836165103645849</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>99.74360353786234</v>
+      </c>
+      <c r="C6" t="n">
+        <v>8.230452674897119</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4.11522633744856</v>
+      </c>
+      <c r="E6" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>64688.6404626334</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.04633071783163444</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>99.73846951877802</v>
+      </c>
+      <c r="C7" t="n">
+        <v>12.86008230452675</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5.1440329218107</v>
+      </c>
+      <c r="E7" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>80944.00083341627</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.06881516250758339</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>99.73204539172772</v>
+      </c>
+      <c r="C8" t="n">
+        <v>18.51851851851852</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6.17283950617284</v>
+      </c>
+      <c r="E8" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.9716506630086876</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>92309.36376947795</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.09445665244354949</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>99.72471925174602</v>
+      </c>
+      <c r="C9" t="n">
+        <v>25.17718335619571</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7.144490169181528</v>
+      </c>
+      <c r="E9" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0.8816830090264018</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>97987.04144175485</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.1216752750662592</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>99.71694250242525</v>
+      </c>
+      <c r="C10" t="n">
+        <v>32.76251502989044</v>
+      </c>
+      <c r="D10" t="n">
+        <v>8.02617317820793</v>
+      </c>
+      <c r="E10" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0.8000456933758091</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>101081.4420481137</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.1497534534129574</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>99.70892016575478</v>
+      </c>
+      <c r="C11" t="n">
+        <v>41.18871105478627</v>
+      </c>
+      <c r="D11" t="n">
+        <v>8.826218871583739</v>
+      </c>
+      <c r="E11" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0.7442224083688047</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>104463.2727333196</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.1787710291722129</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>99.70062942982356</v>
+      </c>
+      <c r="C12" t="n">
+        <v>50.38704113055441</v>
+      </c>
+      <c r="D12" t="n">
+        <v>9.570441279952544</v>
+      </c>
+      <c r="E12" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>0.7028767190149822</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>67147.86387781269</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.1974232135827164</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>99.69530023427771</v>
+      </c>
+      <c r="C13" t="n">
+        <v>60.30892077001444</v>
+      </c>
+      <c r="D13" t="n">
+        <v>10.27331799896753</v>
+      </c>
+      <c r="E13" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>0.6638280124030387</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>65305.45819627993</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.2155636186372386</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>99.69011726140499</v>
+      </c>
+      <c r="C14" t="n">
+        <v>70.91415277518348</v>
+      </c>
+      <c r="D14" t="n">
+        <v>10.93714601137057</v>
+      </c>
+      <c r="E14" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0.6269486783806476</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>151428.2202920164</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.2576270131627987</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>99.6780991486834</v>
+      </c>
+      <c r="C15" t="n">
+        <v>82.16477312574438</v>
+      </c>
+      <c r="D15" t="n">
+        <v>11.56409468975121</v>
+      </c>
+      <c r="E15" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>0.6091420889097003</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>157524.8125526304</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.3013839055385293</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>99.66559717943321</v>
+      </c>
+      <c r="C16" t="n">
+        <v>94.03343885995044</v>
+      </c>
+      <c r="D16" t="n">
+        <v>12.17323677866091</v>
+      </c>
+      <c r="E16" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F16" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>0.598193456592696</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>224426.0499971094</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.3637244749821708</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>99.6477855881636</v>
+      </c>
+      <c r="C17" t="n">
+        <v>106.5057723669077</v>
+      </c>
+      <c r="D17" t="n">
+        <v>12.77143023525361</v>
+      </c>
+      <c r="E17" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F17" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>0.5874416134186443</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>254838.62966634</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.4345129832228208</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Zeit [s]</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>SoC [%]</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Zurückgelegte Distanz [m]</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Ist-Geschwindigkeit zum Zeitpunkt t [m/s]</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Soll-Geschwindigkeit zum Zeitpunkt t [m/s]</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Steigung im Intervall [t, t+1) [%]</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Gewählte Beschleunigung im Intervall [t, t+1) [m/s²]</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Abgerufene Batterieleistung im Intervall [t, t+1) [W]</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Kumulierter Energieverbrauch nach Intervall [t, t+1) [kWh]</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>99.62756030009484</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>37.89473684210527</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1.052631578947369e-05</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>99.62755729257604</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.5144032921810699</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.02880658436214</v>
+      </c>
+      <c r="E3" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>17019.3250964519</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.004738116620359448</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>99.62620655248901</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.05761316872428</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2.05761316872428</v>
+      </c>
+      <c r="E4" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>34013.11198130637</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.01418620328183344</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>99.62350709915717</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4.62962962962963</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3.08641975308642</v>
+      </c>
+      <c r="E5" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>51031.61191665019</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.02836165103645849</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>99.61945697122728</v>
+      </c>
+      <c r="C6" t="n">
+        <v>8.230452674897119</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4.11522633744856</v>
+      </c>
+      <c r="E6" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>64688.6404626334</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.04633071783163444</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>99.61432295214296</v>
+      </c>
+      <c r="C7" t="n">
+        <v>12.86008230452675</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5.1440329218107</v>
+      </c>
+      <c r="E7" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1.02880658436214</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>80944.00083341627</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.06881516250758339</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>99.60789882509268</v>
+      </c>
+      <c r="C8" t="n">
+        <v>18.51851851851852</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6.17283950617284</v>
+      </c>
+      <c r="E8" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.9716506630086876</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>92309.36376947795</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.09445665244354949</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>99.60057268511096</v>
+      </c>
+      <c r="C9" t="n">
+        <v>25.17718335619571</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7.144490169181528</v>
+      </c>
+      <c r="E9" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0.8816830090264018</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>97987.04144175485</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.1216752750662592</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>99.59279593579021</v>
+      </c>
+      <c r="C10" t="n">
+        <v>32.76251502989044</v>
+      </c>
+      <c r="D10" t="n">
+        <v>8.02617317820793</v>
+      </c>
+      <c r="E10" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0.8000456933758091</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>101081.4420481137</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.1497534534129574</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>99.58477359911973</v>
+      </c>
+      <c r="C11" t="n">
+        <v>41.18871105478627</v>
+      </c>
+      <c r="D11" t="n">
+        <v>8.826218871583739</v>
+      </c>
+      <c r="E11" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0.7442224083688047</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>104463.2727333196</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.1787710291722129</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>99.5764828631885</v>
+      </c>
+      <c r="C12" t="n">
+        <v>50.38704113055441</v>
+      </c>
+      <c r="D12" t="n">
+        <v>9.570441279952544</v>
+      </c>
+      <c r="E12" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>0.7028767190149822</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>67147.86387781269</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.1974232135827164</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>99.57115366764265</v>
+      </c>
+      <c r="C13" t="n">
+        <v>60.30892077001444</v>
+      </c>
+      <c r="D13" t="n">
+        <v>10.27331799896753</v>
+      </c>
+      <c r="E13" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>0.6638280124030387</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>65305.45819627993</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.2155636186372386</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>99.56597069476993</v>
+      </c>
+      <c r="C14" t="n">
+        <v>70.91415277518348</v>
+      </c>
+      <c r="D14" t="n">
+        <v>10.93714601137057</v>
+      </c>
+      <c r="E14" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0.6269486783806476</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>151428.2202920164</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.2576270131627987</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>99.55395258204834</v>
+      </c>
+      <c r="C15" t="n">
+        <v>82.16477312574438</v>
+      </c>
+      <c r="D15" t="n">
+        <v>11.56409468975121</v>
+      </c>
+      <c r="E15" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>0.6091420889097003</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>157524.8125526304</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.3013839055385293</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>99.54145061279814</v>
+      </c>
+      <c r="C16" t="n">
+        <v>94.03343885995044</v>
+      </c>
+      <c r="D16" t="n">
+        <v>12.17323677866091</v>
+      </c>
+      <c r="E16" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F16" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>0.598193456592696</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>224426.0499971094</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.3637244749821708</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>99.52363902152854</v>
+      </c>
+      <c r="C17" t="n">
+        <v>106.5057723669077</v>
+      </c>
+      <c r="D17" t="n">
+        <v>12.77143023525361</v>
+      </c>
+      <c r="E17" t="n">
+        <v>13.88888888888889</v>
+      </c>
+      <c r="F17" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>0.5874416134186443</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>254838.62966634</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.4345129832228208</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>